<commit_message>
SCE 2026-2028 WMP - 3
</commit_message>
<xml_diff>
--- a/WMP26/SCE/WMP26-8_MGRA-SCE-05_Q1-CCUG-WD-Ign-jwm.xlsx
+++ b/WMP26/SCE/WMP26-8_MGRA-SCE-05_Q1-CCUG-WD-Ign-jwm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwm/Work/WEEDS/Calculations/Workpapers/WMP26/SCE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7188F610-DD10-7F4E-A909-AA8B85E8BCA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CD60873-194C-E844-B8DA-DAA1C8B4593D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3140" yWindow="500" windowWidth="24300" windowHeight="17660" activeTab="4" xr2:uid="{7B236B09-ABB7-4B70-B063-2F30C6C73F05}"/>
   </bookViews>
@@ -4497,6 +4497,38 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e45da448-bf9c-43e8-8676-7e88d583ded9" xsi:nil="true"/>
+    <Response_x0020_Date xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">2024-01-22T08:00:00+00:00</Response_x0020_Date>
+    <Received_x0020_Date xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">2024-01-05T08:00:00+00:00</Received_x0020_Date>
+    <Proceeding_x0020_Number xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">A.23-05-010</Proceeding_x0020_Number>
+    <Party xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">MGRA</Party>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Source_x0020_ID xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">324633</Source_x0020_ID>
+    <RcmsModDate xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">1/22/2024 6:17 PM</RcmsModDate>
+    <Friendly_x0020_Name xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
+    <Data_x0020_Request_x0020_Set xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
+    <Description0 xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
+    <Proceeding xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
+    <Response_x0020_Document_x0020_Type xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">Attachment</Response_x0020_Document_x0020_Type>
+    <PublicURL xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">https://edisonintl.sharepoint.com/:x:/t/Public/regpublic/EYaaIpz8h-dBrgNSJgLdxZcBrLDNPp5p0r1PCg1GdS_ihw</PublicURL>
+    <Questions xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">2-1.a-f</Questions>
+    <Access_x0020_Classification xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">Public</Access_x0020_Classification>
+    <SharedWithUsers xmlns="0080267e-90ad-460f-9cb6-60e03307a0da">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4505,7 +4537,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F80E8443A091C6489C59EDF60B52CCAF" ma:contentTypeVersion="35" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="283482aaba29cec93de82bd38decaa67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xmlns:ns3="e45da448-bf9c-43e8-8676-7e88d583ded9" xmlns:ns4="0080267e-90ad-460f-9cb6-60e03307a0da" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b99c9bd826a5ff60ac9864a0c3f563f7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d"/>
@@ -4865,67 +4897,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e45da448-bf9c-43e8-8676-7e88d583ded9" xsi:nil="true"/>
-    <Response_x0020_Date xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">2024-01-22T08:00:00+00:00</Response_x0020_Date>
-    <Received_x0020_Date xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">2024-01-05T08:00:00+00:00</Received_x0020_Date>
-    <Proceeding_x0020_Number xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">A.23-05-010</Proceeding_x0020_Number>
-    <Party xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">MGRA</Party>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Source_x0020_ID xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">324633</Source_x0020_ID>
-    <RcmsModDate xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">1/22/2024 6:17 PM</RcmsModDate>
-    <Friendly_x0020_Name xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
-    <Data_x0020_Request_x0020_Set xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
-    <Description0 xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
-    <Proceeding xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d" xsi:nil="true"/>
-    <Response_x0020_Document_x0020_Type xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">Attachment</Response_x0020_Document_x0020_Type>
-    <PublicURL xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">https://edisonintl.sharepoint.com/:x:/t/Public/regpublic/EYaaIpz8h-dBrgNSJgLdxZcBrLDNPp5p0r1PCg1GdS_ihw</PublicURL>
-    <Questions xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">2-1.a-f</Questions>
-    <Access_x0020_Classification xmlns="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d">Public</Access_x0020_Classification>
-    <SharedWithUsers xmlns="0080267e-90ad-460f-9cb6-60e03307a0da">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74C38C2F-7CEA-4412-9AB0-EEC50273DCAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02B0CFAA-35EE-4A2B-99BF-3F85903EFDFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d"/>
-    <ds:schemaRef ds:uri="e45da448-bf9c-43e8-8676-7e88d583ded9"/>
-    <ds:schemaRef ds:uri="0080267e-90ad-460f-9cb6-60e03307a0da"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B969AC4-AA3A-4174-AC2B-51F3DFC145CB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4945,4 +4917,32 @@
     <ds:schemaRef ds:uri="0080267e-90ad-460f-9cb6-60e03307a0da"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74C38C2F-7CEA-4412-9AB0-EEC50273DCAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02B0CFAA-35EE-4A2B-99BF-3F85903EFDFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="38b3f067-3bac-4c47-a6a5-7c76f83e9b8d"/>
+    <ds:schemaRef ds:uri="e45da448-bf9c-43e8-8676-7e88d583ded9"/>
+    <ds:schemaRef ds:uri="0080267e-90ad-460f-9cb6-60e03307a0da"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>